<commit_message>
Updating ML models' stats
</commit_message>
<xml_diff>
--- a/resources/Summary_Stats.xlsx
+++ b/resources/Summary_Stats.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Analysis Projects\Final Project\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD0C1B0-21BA-44A4-9F3C-72BA101237BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79298317-2EC9-4136-B034-C25C41F04F5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="2220" windowWidth="21600" windowHeight="11400" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
+    <workbookView xWindow="1875" yWindow="1875" windowWidth="21600" windowHeight="11400" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Final ML Models" sheetId="2" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Model</t>
   </si>
@@ -96,13 +97,37 @@
   </si>
   <si>
     <t>W total_bags</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Gradient Boosting</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Conventional</t>
+  </si>
+  <si>
+    <t>Organic</t>
+  </si>
+  <si>
+    <t>Combined</t>
+  </si>
+  <si>
+    <t>W/ Avg_Price</t>
+  </si>
+  <si>
+    <t>W/O Avg_Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +151,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +182,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -180,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -208,6 +247,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -523,11 +573,184 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E548DB6-46E4-4991-AEF9-13BA26A579B2}">
+  <dimension ref="B2:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="21">
+        <v>1</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0.72119999999999995</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="21">
+        <v>1</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0.73029999999999995</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="21">
+        <v>1</v>
+      </c>
+      <c r="J5" s="23">
+        <v>0.70760000000000001</v>
+      </c>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="21">
+        <v>1</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0.81579999999999997</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21">
+        <v>1</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0.80889999999999995</v>
+      </c>
+      <c r="H6" s="19"/>
+      <c r="I6" s="21">
+        <v>1</v>
+      </c>
+      <c r="J6" s="23">
+        <v>0.7903</v>
+      </c>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0.80669999999999997</v>
+      </c>
+      <c r="D7" s="22">
+        <v>0.59570000000000001</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22">
+        <v>0.86890000000000001</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.67830000000000001</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="22">
+        <v>0.80869999999999997</v>
+      </c>
+      <c r="J7" s="23">
+        <v>0.60829999999999995</v>
+      </c>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15D3152-AE2F-4127-AD79-B7C7837831BC}">
   <dimension ref="B2:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add ML model results
</commit_message>
<xml_diff>
--- a/resources/Summary_Stats.xlsx
+++ b/resources/Summary_Stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Analysis Projects\Final Project\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfand\Google Drive\DataAnalytics\ClassWork\M20_GroupProject\GitHubRepo_Colab\Health_and_Avocados\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79298317-2EC9-4136-B034-C25C41F04F5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3EDD6D-C64F-469D-A24F-21416B3BEDA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="1875" windowWidth="21600" windowHeight="11400" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
+    <workbookView xWindow="30270" yWindow="795" windowWidth="21780" windowHeight="12675" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Final ML Models" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
   <si>
     <t>Model</t>
   </si>
@@ -121,6 +121,57 @@
   </si>
   <si>
     <t>W/O Avg_Price</t>
+  </si>
+  <si>
+    <t>Random Forest Regressor</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>R2 = 0.89, mse = 0.01</t>
+  </si>
+  <si>
+    <t>R2=0.83, mse = 0.01</t>
+  </si>
+  <si>
+    <t>R2=0.80, mse = 0.02</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier (4 caregories)</t>
+  </si>
+  <si>
+    <t>Data used: prices &amp; production</t>
+  </si>
+  <si>
+    <t>Linear Regression with sckit-learn</t>
+  </si>
+  <si>
+    <t>R2 = 0.66, mse = 0.04</t>
+  </si>
+  <si>
+    <t>R2 = 0.79, mse = 0.02</t>
+  </si>
+  <si>
+    <t>R2 = 0.78, mse = 0.02</t>
+  </si>
+  <si>
+    <t>Decision Tree Classifier</t>
+  </si>
+  <si>
+    <t>R2=0.88, mse = 0.01</t>
+  </si>
+  <si>
+    <t>R2 = 0.92, mse=0.01</t>
+  </si>
+  <si>
+    <t>R2 = 0.92, mse = 0.01</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier (4 categories)</t>
+  </si>
+  <si>
+    <t>Regions_only</t>
   </si>
 </sst>
 </file>
@@ -192,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -215,11 +266,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -260,6 +337,8 @@
     <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,23 +653,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E548DB6-46E4-4991-AEF9-13BA26A579B2}">
-  <dimension ref="B2:K8"/>
+  <dimension ref="B2:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -729,16 +808,56 @@
       <c r="K7" s="18"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
+      <c r="F8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="H8" s="19"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="19"/>
+      <c r="I8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>33</v>
+      </c>
       <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="21">
+        <v>0.78</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="21">
+        <v>0.69</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="21">
+        <v>0.71</v>
+      </c>
+      <c r="K9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -747,26 +866,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15D3152-AE2F-4127-AD79-B7C7837831BC}">
-  <dimension ref="B2:K22"/>
+  <dimension ref="B2:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K22"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:14" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -782,8 +902,12 @@
         <v>20</v>
       </c>
       <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="2:11" s="1" customFormat="1" ht="52.5" x14ac:dyDescent="0.4">
+      <c r="M2" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="25"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="52.5" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -811,8 +935,14 @@
       <c r="K3" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
@@ -841,7 +971,7 @@
         <v>0.632043116119549</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -854,7 +984,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
@@ -867,7 +997,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
@@ -880,7 +1010,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
@@ -909,7 +1039,7 @@
         <v>0.64805016656868497</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
@@ -938,7 +1068,7 @@
         <v>0.58876367793565199</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -967,7 +1097,7 @@
         <v>0.64805016656868497</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
@@ -996,7 +1126,7 @@
         <v>0.60231912461211801</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>14</v>
       </c>
@@ -1025,7 +1155,7 @@
         <v>0.63787461554142699</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>15</v>
       </c>
@@ -1054,7 +1184,7 @@
         <v>0.63462199531962105</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>16</v>
       </c>
@@ -1083,7 +1213,7 @@
         <v>0.63977865209892903</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>18</v>
       </c>
@@ -1112,7 +1242,7 @@
         <v>0.63008666786991696</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
@@ -1141,7 +1271,7 @@
         <v>0.632939955434629</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1152,60 +1282,164 @@
       <c r="J17" s="4"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="6"/>
-      <c r="H18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="H18" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="6"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="6"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="6"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="6"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="6"/>
+      <c r="K18" s="4"/>
+      <c r="M18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.77031872652664402</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.70198508859502695</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.69582050521723204</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.68957200513993799</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0.70265103123147399</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0.71830093499320902</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.77031872652664402</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.77988166896385602</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.77827746449568103</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0.77725003390482394</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0.80673209414841296</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0.80459159003249203</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cleaned up arima, lstm univariate and multivariate and updated summary and readme
</commit_message>
<xml_diff>
--- a/resources/Summary_Stats.xlsx
+++ b/resources/Summary_Stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfand\Google Drive\DataAnalytics\ClassWork\M20_GroupProject\GitHubRepo_Colab\Health_and_Avocados\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents1\GitHub\Health_and_Avocados\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3EDD6D-C64F-469D-A24F-21416B3BEDA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EE77E1-37F6-4845-A81F-DDBF60577BE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30270" yWindow="795" windowWidth="21780" windowHeight="12675" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
+    <workbookView xWindow="3570" yWindow="3090" windowWidth="33285" windowHeight="19335" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Final ML Models" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
   <si>
     <t>Model</t>
   </si>
@@ -172,6 +172,33 @@
   </si>
   <si>
     <t>Regions_only</t>
+  </si>
+  <si>
+    <t>ARIMA</t>
+  </si>
+  <si>
+    <t>LSTM Univariate</t>
+  </si>
+  <si>
+    <t>Test RMSE = 0.34</t>
+  </si>
+  <si>
+    <t>Test RMSE = 0.33</t>
+  </si>
+  <si>
+    <t>RMSE= 0.34</t>
+  </si>
+  <si>
+    <t>RMSE =  0.21</t>
+  </si>
+  <si>
+    <t>RMSE = 0.27</t>
+  </si>
+  <si>
+    <t>ARIMA with seasonality</t>
+  </si>
+  <si>
+    <t>RMSE =  0.39</t>
   </si>
 </sst>
 </file>
@@ -653,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E548DB6-46E4-4991-AEF9-13BA26A579B2}">
-  <dimension ref="B2:K9"/>
+  <dimension ref="B2:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,6 +885,80 @@
         <v>0.71</v>
       </c>
       <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added brf model accuracy score
</commit_message>
<xml_diff>
--- a/resources/Summary_Stats.xlsx
+++ b/resources/Summary_Stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents1\GitHub\Health_and_Avocados\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amelin\GitHubRepos\Health_and_Avocados\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EE77E1-37F6-4845-A81F-DDBF60577BE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6FAB35-6A82-4E68-832D-6EE50FD3F169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="3090" windowWidth="33285" windowHeight="19335" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Final ML Models" sheetId="2" r:id="rId1"/>
@@ -33,8 +33,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Amelin</author>
+  </authors>
+  <commentList>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{126B8753-7AA7-4557-9AB7-9B55A991B22B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amelin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+prices_clim dataset</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{8C340220-5F68-4096-80DC-365734D23A19}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Amelin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+prices_prod dataset</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
   <si>
     <t>Model</t>
   </si>
@@ -138,9 +196,6 @@
     <t>R2=0.80, mse = 0.02</t>
   </si>
   <si>
-    <t>Random Forest Classifier (4 caregories)</t>
-  </si>
-  <si>
     <t>Data used: prices &amp; production</t>
   </si>
   <si>
@@ -199,13 +254,19 @@
   </si>
   <si>
     <t>RMSE =  0.39</t>
+  </si>
+  <si>
+    <t>Balanced Random Forest Classifier (qcut into 3 categories)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +297,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -323,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -359,13 +433,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,28 +766,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E548DB6-46E4-4991-AEF9-13BA26A579B2}">
-  <dimension ref="B2:K12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E548DB6-46E4-4991-AEF9-13BA26A579B2}">
+  <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>26</v>
@@ -718,7 +805,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -744,7 +831,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="17"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -756,212 +843,249 @@
       <c r="J4" s="19"/>
       <c r="K4" s="18"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="23">
         <v>1</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="24">
         <v>0.72119999999999995</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="21">
+      <c r="E5" s="24"/>
+      <c r="F5" s="23">
         <v>1</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="25">
         <v>0.73029999999999995</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="21">
+      <c r="H5" s="26"/>
+      <c r="I5" s="23">
         <v>1</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="25">
         <v>0.70760000000000001</v>
       </c>
       <c r="K5" s="18"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="23">
         <v>1</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="24">
         <v>0.81579999999999997</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="21">
+      <c r="E6" s="24"/>
+      <c r="F6" s="23">
         <v>1</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="25">
         <v>0.80889999999999995</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="21">
+      <c r="H6" s="26"/>
+      <c r="I6" s="23">
         <v>1</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="25">
         <v>0.7903</v>
       </c>
       <c r="K6" s="18"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="24">
         <v>0.80669999999999997</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="24">
         <v>0.59570000000000001</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24">
         <v>0.86890000000000001</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="25">
         <v>0.67830000000000001</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="22">
+      <c r="H7" s="26"/>
+      <c r="I7" s="24">
         <v>0.80869999999999997</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="25">
         <v>0.60829999999999995</v>
       </c>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="18" t="s">
+      <c r="E8" s="27"/>
+      <c r="F8" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="18" t="s">
+      <c r="H8" s="26"/>
+      <c r="I8" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="27" t="s">
         <v>33</v>
       </c>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="21">
+        <v>43</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="23">
         <v>0.78</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="21">
+      <c r="E9" s="28"/>
+      <c r="F9" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="23">
         <v>0.69</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="21">
+      <c r="H9" s="28"/>
+      <c r="I9" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="23">
         <v>0.71</v>
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="23">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="28"/>
+      <c r="I10" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="21">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="21" t="s">
+      <c r="C11" s="27"/>
+      <c r="D11" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="28"/>
+      <c r="I11" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="28"/>
+      <c r="I12" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="21" t="s">
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="4"/>
+      <c r="C13" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="24">
+        <v>0.82802571940671299</v>
+      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="24">
+        <v>0.82032054041787095</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -973,21 +1097,21 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:14" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -1003,12 +1127,12 @@
         <v>20</v>
       </c>
       <c r="K2" s="5"/>
-      <c r="M2" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" s="25"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="52.5" x14ac:dyDescent="0.4">
+      <c r="M2" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="22"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="51.6" x14ac:dyDescent="0.5">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
@@ -1072,7 +1196,7 @@
         <v>0.632043116119549</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1085,7 +1209,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1098,7 +1222,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1111,7 +1235,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1140,7 +1264,7 @@
         <v>0.64805016656868497</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1293,7 @@
         <v>0.58876367793565199</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1198,7 +1322,7 @@
         <v>0.64805016656868497</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1227,7 +1351,7 @@
         <v>0.60231912461211801</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>14</v>
       </c>
@@ -1256,7 +1380,7 @@
         <v>0.63787461554142699</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
         <v>15</v>
       </c>
@@ -1285,7 +1409,7 @@
         <v>0.63462199531962105</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>16</v>
       </c>
@@ -1314,7 +1438,7 @@
         <v>0.63977865209892903</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
         <v>18</v>
       </c>
@@ -1343,7 +1467,7 @@
         <v>0.63008666786991696</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
@@ -1372,7 +1496,7 @@
         <v>0.632939955434629</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1383,63 +1507,63 @@
       <c r="J17" s="4"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="H18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N18" s="4"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19" s="4" t="s">
+      <c r="N19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N19" s="4" t="s">
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C20" s="4">
         <v>0.77031872652664402</v>
@@ -1472,7 +1596,7 @@
         <v>0.71830093499320902</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>29</v>
       </c>
@@ -1480,7 +1604,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>30</v>
@@ -1492,24 +1616,24 @@
         <v>31</v>
       </c>
       <c r="I21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M21" s="4" t="s">
+      <c r="N21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N21" s="4" t="s">
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C22" s="4">
         <v>0.77031872652664402</v>

</xml_diff>

<commit_message>
added resources to readme and updated summary stats
</commit_message>
<xml_diff>
--- a/resources/Summary_Stats.xlsx
+++ b/resources/Summary_Stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents1\GitHub\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents1\GitHub\Health_and_Avocados\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F0BEC81-D455-49A1-A609-7F319CCC5C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E312E0E-A5CA-4716-88C7-7B0A308CAF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23730" yWindow="3540" windowWidth="33285" windowHeight="19335" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
+    <workbookView xWindow="9375" yWindow="1665" windowWidth="33285" windowHeight="19335" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Final ML Models" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Amelin</author>
   </authors>
   <commentList>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{126B8753-7AA7-4557-9AB7-9B55A991B22B}">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{126B8753-7AA7-4557-9AB7-9B55A991B22B}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{8C340220-5F68-4096-80DC-365734D23A19}">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{8C340220-5F68-4096-80DC-365734D23A19}">
       <text>
         <r>
           <rPr>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
   <si>
     <t>Model</t>
   </si>
@@ -250,9 +250,6 @@
     <t>RMSE = 0.27</t>
   </si>
   <si>
-    <t>ARIMA with seasonality</t>
-  </si>
-  <si>
     <t>Balanced Random Forest Classifier (qcut into 3 categories)</t>
   </si>
   <si>
@@ -260,12 +257,6 @@
   </si>
   <si>
     <t>RMSE = 0.29</t>
-  </si>
-  <si>
-    <t>RMSE =  0.26</t>
-  </si>
-  <si>
-    <t>RMSE = 0.38</t>
   </si>
   <si>
     <t>lSTM Multivariate with lags</t>
@@ -788,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E548DB6-46E4-4991-AEF9-13BA26A579B2}">
-  <dimension ref="B2:K15"/>
+  <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,7 +993,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="27" t="s">
@@ -1046,61 +1037,55 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="23"/>
+        <v>55</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="23" t="s">
+        <v>56</v>
+      </c>
       <c r="E12" s="28"/>
       <c r="F12" s="27" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H12" s="28"/>
       <c r="I12" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="27" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>59</v>
       </c>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="23" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="24">
+        <v>0.82802571940671299</v>
       </c>
       <c r="E13" s="28"/>
-      <c r="F13" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>60</v>
-      </c>
+      <c r="F13" s="27"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="28"/>
-      <c r="I13" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>62</v>
-      </c>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="27" t="s">
-        <v>54</v>
-      </c>
       <c r="D14" s="24">
-        <v>0.82802571940671299</v>
+        <v>0.82032054041787095</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="27"/>
@@ -1109,24 +1094,6 @@
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
       <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="24">
-        <v>0.82032054041787095</v>
-      </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating the files correctly
</commit_message>
<xml_diff>
--- a/resources/Summary_Stats.xlsx
+++ b/resources/Summary_Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\git\Health_and_Avocados\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA812435-3406-4EB3-B7FA-E21EC02EDA2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE458FB9-DC26-4ABE-A38F-00F82F7ECA7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="1680" windowWidth="21600" windowHeight="11400" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
   </bookViews>
@@ -752,7 +752,7 @@
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +803,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="24">
-        <v>0.82802571940671299</v>
+        <v>0.88</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="23"/>
@@ -811,10 +811,10 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C6" s="24">
-        <v>0.82032054041787095</v>
+        <v>0.85</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="23"/>

</xml_diff>

<commit_message>
improvements to model and updated readme
</commit_message>
<xml_diff>
--- a/resources/Summary_Stats.xlsx
+++ b/resources/Summary_Stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\git\Health_and_Avocados\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents1\GitHub\Health_and_Avocados\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF2D28D-E4C2-4B6F-902D-B69D0ECD7E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405A9391-3E3E-416F-960F-AE8BFDAEC2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1680" windowWidth="21600" windowHeight="11400" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
+    <workbookView xWindow="16380" yWindow="2505" windowWidth="33285" windowHeight="19335" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Final ML Models" sheetId="2" r:id="rId1"/>
@@ -235,16 +235,16 @@
     <t>RMSE = 0.29</t>
   </si>
   <si>
-    <t>lSTM Multivariate with lags</t>
-  </si>
-  <si>
-    <t>RMSE= 0.221</t>
-  </si>
-  <si>
-    <t>RMSE= 0.162 (With 3 lags)</t>
-  </si>
-  <si>
-    <t>RMSE= 0.167 (With 3 lags)</t>
+    <t>lSTM Multivariate with 1 lag</t>
+  </si>
+  <si>
+    <t>RMSE= 0.094</t>
+  </si>
+  <si>
+    <t>RMSE= 0.054</t>
+  </si>
+  <si>
+    <t>RMSE= 0.095</t>
   </si>
 </sst>
 </file>
@@ -740,7 +740,7 @@
   <dimension ref="B2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,13 +823,13 @@
         <v>47</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>